<commit_message>
updated LoginManager test sheet with results; changed vision scope doc name and edits
</commit_message>
<xml_diff>
--- a/test_cases/stqa_NEW/LoginManagerTesting.xlsx
+++ b/test_cases/stqa_NEW/LoginManagerTesting.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CheckPasswordUnit" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="66">
   <si>
     <t>test #</t>
   </si>
@@ -208,6 +208,12 @@
   </si>
   <si>
     <t>LoginManagerUnitTesting.cs</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
@@ -260,7 +266,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -270,12 +276,146 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -574,8 +714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,6 +805,12 @@
       <c r="F6" t="b">
         <v>1</v>
       </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -685,6 +831,12 @@
       <c r="F7" t="b">
         <v>0</v>
       </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -705,6 +857,12 @@
       <c r="F8" t="b">
         <v>0</v>
       </c>
+      <c r="G8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -754,6 +912,12 @@
       <c r="F13" t="b">
         <v>0</v>
       </c>
+      <c r="G13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -768,6 +932,12 @@
       <c r="F14" t="b">
         <v>0</v>
       </c>
+      <c r="G14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -782,6 +952,12 @@
       <c r="F15" t="b">
         <v>0</v>
       </c>
+      <c r="G15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -795,6 +971,12 @@
       </c>
       <c r="F16" t="b">
         <v>0</v>
+      </c>
+      <c r="G16" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -804,6 +986,16 @@
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
   </mergeCells>
+  <conditionalFormatting sqref="H6:H8">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",H6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H13:H16">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",H13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -813,8 +1005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,7 +1014,8 @@
     <col min="1" max="1" width="9.7109375" customWidth="1"/>
     <col min="2" max="2" width="17.140625" customWidth="1"/>
     <col min="3" max="3" width="41.5703125" customWidth="1"/>
-    <col min="4" max="5" width="27.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
     <col min="6" max="6" width="28.5703125" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
     <col min="8" max="8" width="14.7109375" customWidth="1"/>
@@ -845,9 +1038,10 @@
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
-      <c r="E2" t="s">
+      <c r="E2" s="5" t="s">
         <v>63</v>
       </c>
+      <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
@@ -918,6 +1112,12 @@
       <c r="H6" t="b">
         <v>0</v>
       </c>
+      <c r="I6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -944,6 +1144,12 @@
       <c r="H7" t="b">
         <v>1</v>
       </c>
+      <c r="I7" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
@@ -1005,6 +1211,12 @@
       <c r="H11" t="b">
         <v>1</v>
       </c>
+      <c r="I11" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1028,6 +1240,12 @@
       <c r="H12" t="b">
         <v>1</v>
       </c>
+      <c r="I12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -1049,6 +1267,12 @@
       <c r="H13" t="b">
         <v>0</v>
       </c>
+      <c r="I13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J13" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1069,6 +1293,12 @@
       <c r="H14" t="b">
         <v>0</v>
       </c>
+      <c r="I14" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -1086,17 +1316,40 @@
       <c r="H15" t="b">
         <v>0</v>
       </c>
+      <c r="I15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" t="s">
+        <v>65</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
+    <mergeCell ref="E2:F2"/>
   </mergeCells>
+  <conditionalFormatting sqref="J11:J15">
+    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",J11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="3" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",J11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J6:J7">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",J6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",J6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="F7" r:id="rId1"/>
-    <hyperlink ref="F11"/>
+    <hyperlink ref="F11" display="lucifer00666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666666"/>
     <hyperlink ref="F12" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>